<commit_message>
Updated Requirements with feedback from DVConUS2021 workshop
</commit_message>
<xml_diff>
--- a/doc/RequirementsRandomization.xlsx
+++ b/doc/RequirementsRandomization.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\gitrepositories\voertler-crave\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD9DBEE8-78C1-4A0A-A0D7-0B66A2EC5D55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C05E2A-60E4-45A1-874C-98B24437087A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRV" sheetId="1" r:id="rId1"/>
     <sheet name="CRV.Class" sheetId="13" r:id="rId2"/>
     <sheet name="CRV.DataTypes" sheetId="17" r:id="rId3"/>
     <sheet name="CRV.Phases" sheetId="18" r:id="rId4"/>
-    <sheet name="Top.B" sheetId="14" r:id="rId5"/>
-    <sheet name="Top.A.X" sheetId="15" r:id="rId6"/>
-    <sheet name="Top.A.Y" sheetId="16" r:id="rId7"/>
+    <sheet name="CRV.Constraints" sheetId="19" r:id="rId5"/>
+    <sheet name="CRV.General" sheetId="20" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" iterateCount="5"/>
   <extLst>
@@ -574,8 +573,280 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Khundakjie, Faris H</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D0997DF9-AEEA-4C42-9908-8DA40AE16BFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Succinct requirement decsription</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{E60E5074-46AE-4D6D-8E7B-D71A97B8DE1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Why requirement exists</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{A85B8C63-BAB8-4058-B238-BF77CE327992}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>higher level requirement this requirement is considered to be a sub-requirement of</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{E817E76F-D632-4B7D-94AC-15429566661E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Next level sub-requirement that this requirement is considered to be a parent or the architectural component(s) that this last sub level requirement maps to</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{46C6CF32-503D-4C54-96F5-BA7C45EA0E8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Likelihood requirement will not change</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{7AA43586-918B-4DAD-9A10-54C83431F020}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Extent to which this requirement interacts with other requirements or results in architectural changes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{17920DED-A8EF-4AB3-B428-CA0B98A39117}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Importance of meeting this requirement in order relative to other requirements</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{03AA1274-D536-4D9D-B0D1-6094BB836195}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nature of requirement as a functional requirement vs non-functional, quantifiable vs non-quantifiable, emerging vs non-emerging, process vs non-emerging</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{69EC15B7-5F32-41A7-BC4C-8125A5C9B315}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stakeholders that contributed the requirement</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Khundakjie, Faris H</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{767E464E-5034-4DB4-8013-ACFD8FD04488}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Succinct requirement decsription</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{13EC91ED-6559-4B71-9D74-CD2A9B68D6F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Why requirement exists</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{447BEE6A-0045-4215-91F6-F42EAB1EFFAB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>higher level requirement this requirement is considered to be a sub-requirement of</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{F1B394B8-A9EB-42D6-9F4C-8EEBFE8968CF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Next level sub-requirement that this requirement is considered to be a parent or the architectural component(s) that this last sub level requirement maps to</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{1E19CD1F-7CBF-4C7D-991D-C30A886B100F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Likelihood requirement will not change</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{C5D451CB-3D05-46F8-8CC9-91BE1BE1932D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Extent to which this requirement interacts with other requirements or results in architectural changes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{30352ED9-0B69-4240-B97B-27A244DE4BB7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Importance of meeting this requirement in order relative to other requirements</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{112D9C7C-508C-4897-83A7-C236A8E50F25}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nature of requirement as a functional requirement vs non-functional, quantifiable vs non-quantifiable, emerging vs non-emerging, process vs non-emerging</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{6432CADC-B2AA-4894-A7B0-67DDA2084320}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stakeholders that contributed the requirement</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="118">
   <si>
     <t>Rationale</t>
   </si>
@@ -804,9 +1075,6 @@
     <t>Class.3</t>
   </si>
   <si>
-    <t>Class.1, Class.2, Class.3</t>
-  </si>
-  <si>
     <t>Support non-fixed SystemC Datatypes i.e. sc_bv&lt;&gt; , sc_int&lt;&gt;, sc_uint&lt;&gt;</t>
   </si>
   <si>
@@ -840,9 +1108,6 @@
     <t>DataTypes.4</t>
   </si>
   <si>
-    <t xml:space="preserve">Real values are used SystemC AMS modelling </t>
-  </si>
-  <si>
     <t>Support a randomizable enum type</t>
   </si>
   <si>
@@ -858,18 +1123,12 @@
     <t>These are standard digital datatypes with bitlevel support for SystemC</t>
   </si>
   <si>
-    <t>Analaog / Real value verification</t>
-  </si>
-  <si>
     <t>Verification of Software</t>
   </si>
   <si>
     <t>Easier description  of FSM states</t>
   </si>
   <si>
-    <t>DataTypes.1, DataTypes.2, DataTypes.3, DataTypes.4</t>
-  </si>
-  <si>
     <t>Phases.1</t>
   </si>
   <si>
@@ -877,6 +1136,97 @@
   </si>
   <si>
     <t>Also the DUT can be randomized with constraints e.g. for design exploration or parameter variations</t>
+  </si>
+  <si>
+    <t>DataTypes.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support fixed point datatypes </t>
+  </si>
+  <si>
+    <t>Extension to fixed point demantic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVCON US 2021 Tutorial Remark </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog / Real value verification
+Also in Discusstion for UVM AMS on SystemVerilog </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real values are used AMS (SystemC AMS)modelling </t>
+  </si>
+  <si>
+    <t>Support randomization using constraints</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Support for constraints</t>
+  </si>
+  <si>
+    <t>Constraints.1</t>
+  </si>
+  <si>
+    <t>Support for soft constraints</t>
+  </si>
+  <si>
+    <t>All kinds of randomization</t>
+  </si>
+  <si>
+    <t>CRV.Datatypes</t>
+  </si>
+  <si>
+    <t>CRV.Class</t>
+  </si>
+  <si>
+    <t>CRV.Phases</t>
+  </si>
+  <si>
+    <t>CRV.Constraints</t>
+  </si>
+  <si>
+    <t>Phases.2</t>
+  </si>
+  <si>
+    <t>Support pre_randomize() and post_randomize() callback</t>
+  </si>
+  <si>
+    <t>Enables callback for pre and post randomization</t>
+  </si>
+  <si>
+    <t>Constraints.2</t>
+  </si>
+  <si>
+    <t>Ability to Debug conflicting constraints</t>
+  </si>
+  <si>
+    <t>Enables the ability to add  constraints whcih can be dropped to avoid overconstrainging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSEDA, DVCON US 2021 Tutorial Remark </t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>General Requirements which are not part of other sections</t>
+  </si>
+  <si>
+    <t>CRV.General</t>
+  </si>
+  <si>
+    <t>More complex constraints</t>
+  </si>
+  <si>
+    <t>Conflicting constraints can easily occur</t>
+  </si>
+  <si>
+    <t>General.1</t>
+  </si>
+  <si>
+    <t>Support for randomization with reproducable results (e.g. based on a seed)</t>
   </si>
 </sst>
 </file>
@@ -886,7 +1236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -917,6 +1267,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1079,7 +1435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1144,6 +1500,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,35 +1786,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.453125" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="11" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="6" max="6" width="21.81640625" customWidth="1"/>
+    <col min="7" max="7" width="22.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="10" max="11" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">TODAY()</f>
-        <v>44258</v>
+        <v>44259</v>
       </c>
       <c r="D2" s="3"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1465,12 +1824,12 @@
       <c r="D3" s="3"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="D4" s="3"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1846,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -1506,7 +1865,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="13"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
@@ -1525,7 +1884,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
@@ -1544,7 +1903,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
@@ -1563,7 +1922,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
@@ -1582,7 +1941,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1601,7 +1960,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1979,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>16</v>
       </c>
@@ -1639,7 +1998,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -1654,12 +2013,12 @@
       <c r="L14" s="19"/>
       <c r="M14" s="20"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
       <c r="D15" s="3"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1676,7 +2035,7 @@
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1695,7 +2054,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="13"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
         <v>20</v>
@@ -1712,7 +2071,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>21</v>
       </c>
@@ -1731,7 +2090,7 @@
       <c r="L19" s="17"/>
       <c r="M19" s="18"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
         <v>23</v>
@@ -1748,7 +2107,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
@@ -1767,7 +2126,7 @@
       <c r="L21" s="17"/>
       <c r="M21" s="18"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
@@ -1786,12 +2145,12 @@
       <c r="L22" s="17"/>
       <c r="M22" s="18"/>
     </row>
-    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>2</v>
       </c>
@@ -1826,7 +2185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>63</v>
       </c>
@@ -1841,7 +2200,7 @@
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="23" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
@@ -1851,7 +2210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
         <v>62</v>
       </c>
@@ -1866,7 +2225,7 @@
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="30" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1876,7 +2235,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>58</v>
       </c>
@@ -1884,46 +2243,70 @@
         <v>59</v>
       </c>
       <c r="C30" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="23" t="s">
-        <v>70</v>
-      </c>
       <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
+      <c r="F30" s="22" t="s">
+        <v>102</v>
+      </c>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="K30" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>99</v>
+      </c>
       <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
+      <c r="F31" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="23"/>
+      <c r="K31" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>112</v>
+      </c>
       <c r="C32" s="23"/>
       <c r="D32" s="23"/>
       <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
+      <c r="F32" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="24"/>
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
@@ -1936,7 +2319,7 @@
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="22"/>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
@@ -1949,7 +2332,7 @@
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="22"/>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -1962,7 +2345,7 @@
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="22"/>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
@@ -1975,7 +2358,7 @@
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="22"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -1988,7 +2371,7 @@
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="22"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
@@ -2001,7 +2384,7 @@
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="22"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
@@ -2014,7 +2397,7 @@
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="22"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
@@ -2027,7 +2410,7 @@
       <c r="J40" s="22"/>
       <c r="K40" s="22"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="22"/>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
@@ -2040,7 +2423,7 @@
       <c r="J41" s="22"/>
       <c r="K41" s="22"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="22"/>
       <c r="B42" s="23"/>
       <c r="C42" s="23"/>
@@ -2053,7 +2436,7 @@
       <c r="J42" s="22"/>
       <c r="K42" s="22"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="22"/>
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
@@ -2081,16 +2464,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
-    <col min="4" max="4" width="54.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="56.453125" customWidth="1"/>
+    <col min="3" max="3" width="43.81640625" customWidth="1"/>
+    <col min="4" max="4" width="54.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -2125,7 +2508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>65</v>
       </c>
@@ -2145,7 +2528,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>64</v>
       </c>
@@ -2165,7 +2548,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>66</v>
       </c>
@@ -2193,22 +2576,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036F88FA-F07A-47B0-9FC3-1F5195445874}">
-  <dimension ref="A2:K7"/>
+  <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -2243,90 +2626,108 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" t="s">
         <v>74</v>
       </c>
-      <c r="K3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="26" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
         <v>79</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" t="s">
         <v>74</v>
       </c>
-      <c r="K7" t="s">
-        <v>75</v>
+    </row>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -2337,19 +2738,19 @@
   <dimension ref="A2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -2384,40 +2785,49 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s">
         <v>74</v>
       </c>
-      <c r="K3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="26"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="25"/>
       <c r="C5" s="28"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="25"/>
       <c r="C6" s="27"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="25"/>
       <c r="C7" s="28"/>
       <c r="D7" s="1"/>
@@ -2429,37 +2839,204 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DC5BC3-1009-41D0-BFCB-1714155A6510}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BD1E44-B9B8-49AF-8741-2189991CFC44}">
+  <dimension ref="A2:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="25"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B68C0C-F007-4DF4-A9E5-4E697FC8F37C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A58B5F-9032-4A34-BED6-F46AB697F1B6}">
+  <dimension ref="A2:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="25"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="25"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BB66CD-64D5-4D54-ABFD-55E50195804E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>